<commit_message>
update with August 10th data
</commit_message>
<xml_diff>
--- a/Covid-19.xlsx
+++ b/Covid-19.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2830" documentId="11_E0DBB201481B1C811047287C66E952F5F4A270EB" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{EFEC6F34-29C4-45E3-A9A1-D056D5164523}"/>
   <bookViews>
-    <workbookView xWindow="16690" yWindow="-350" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16690" yWindow="-350" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="International" sheetId="1" r:id="rId1"/>
@@ -2463,17 +2463,17 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2542,17 +2542,17 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000000%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000%"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000000%"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -9087,10 +9087,10 @@
     <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="% Active" totalsRowDxfId="2">
       <calculatedColumnFormula>Table1[[#This Row],[Active]]/Table1[[#This Row],[Cases]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C5BC61F0-787C-4B13-B094-7F65C2839684}" name="Percent Actively Infected" dataDxfId="20" totalsRowDxfId="1">
+    <tableColumn id="4" xr3:uid="{C5BC61F0-787C-4B13-B094-7F65C2839684}" name="Percent Actively Infected" dataDxfId="22" totalsRowDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[Percent Infected]]*Table1[[#This Row],[% Active]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C200E07E-202A-4F23-AD30-2B5D0B3475C7}" name="1/# Active" dataDxfId="19" totalsRowDxfId="0">
+    <tableColumn id="6" xr3:uid="{C200E07E-202A-4F23-AD30-2B5D0B3475C7}" name="1/# Active" dataDxfId="21" totalsRowDxfId="0">
       <calculatedColumnFormula>1/Table1[[#This Row],[Percent Actively Infected]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9129,10 +9129,10 @@
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Percent Dead"/>
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Percent Ex(Death)"/>
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Cases per Test"/>
-    <tableColumn id="23" xr3:uid="{9B168E7D-9EBA-4A79-8254-0356C277894C}" name="Percent Active Infected" dataDxfId="22">
+    <tableColumn id="23" xr3:uid="{9B168E7D-9EBA-4A79-8254-0356C277894C}" name="Percent Active Infected" dataDxfId="20">
       <calculatedColumnFormula>Table2[[#This Row],[Percent Infected]]*Table2[[#This Row],[% Active]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{6B6B44B4-3DE3-4BD0-979D-79BA94F42EB9}" name="1/# Active" dataDxfId="21">
+    <tableColumn id="24" xr3:uid="{6B6B44B4-3DE3-4BD0-979D-79BA94F42EB9}" name="1/# Active" dataDxfId="19">
       <calculatedColumnFormula>1/Table2[[#This Row],[Percent Active Infected]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -25653,11 +25653,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMI91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="13" ySplit="17" topLeftCell="N59" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="13" ySplit="17" topLeftCell="N18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30746,13 +30746,13 @@
       <c r="B61" s="65">
         <v>9308</v>
       </c>
-      <c r="C61" s="83">
+      <c r="C61" s="81">
         <v>15</v>
       </c>
       <c r="D61" s="66">
         <v>472</v>
       </c>
-      <c r="E61" s="84">
+      <c r="E61" s="82">
         <v>2</v>
       </c>
       <c r="F61" s="65">
@@ -34069,14 +34069,14 @@
         <f t="shared" si="9"/>
         <v>1.0370383454624368</v>
       </c>
-      <c r="H147" s="82" t="s">
+      <c r="H147" s="84" t="s">
         <v>306</v>
       </c>
-      <c r="I147" s="82"/>
-      <c r="J147" s="82"/>
-      <c r="K147" s="82"/>
-      <c r="L147" s="82"/>
-      <c r="M147" s="82"/>
+      <c r="I147" s="84"/>
+      <c r="J147" s="84"/>
+      <c r="K147" s="84"/>
+      <c r="L147" s="84"/>
+      <c r="M147" s="84"/>
     </row>
     <row r="148" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B148" s="35">
@@ -34096,10 +34096,10 @@
         <f t="shared" si="9"/>
         <v>1.1397876037845143</v>
       </c>
-      <c r="H148" s="81" t="s">
+      <c r="H148" s="83" t="s">
         <v>308</v>
       </c>
-      <c r="I148" s="81"/>
+      <c r="I148" s="83"/>
       <c r="J148" t="s">
         <v>309</v>
       </c>
@@ -34537,14 +34537,14 @@
         <f>SUM(D$2:D161)</f>
         <v>5617036.9023065362</v>
       </c>
-      <c r="H161" s="82" t="s">
+      <c r="H161" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="I161" s="82"/>
-      <c r="J161" s="82"/>
-      <c r="K161" s="82"/>
-      <c r="L161" s="82"/>
-      <c r="M161" s="82"/>
+      <c r="I161" s="84"/>
+      <c r="J161" s="84"/>
+      <c r="K161" s="84"/>
+      <c r="L161" s="84"/>
+      <c r="M161" s="84"/>
     </row>
     <row r="162" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B162" s="35">
@@ -36963,7 +36963,7 @@
         <v>12.528156753134573</v>
       </c>
       <c r="D268" s="39">
-        <f t="shared" ref="D268:D324" si="15">D267*AVERAGE($F$144:$F$150)</f>
+        <f t="shared" ref="D268:D294" si="15">D267*AVERAGE($F$144:$F$150)</f>
         <v>462.06445959389265</v>
       </c>
       <c r="E268" s="37">
@@ -37211,7 +37211,7 @@
         <v>44182</v>
       </c>
       <c r="C280" s="39">
-        <f t="shared" ref="C280:C324" si="16">$E$150*D266</f>
+        <f t="shared" ref="C280:C294" si="16">$E$150*D266</f>
         <v>7.8154610987663959</v>
       </c>
       <c r="D280" s="39">
@@ -37773,7 +37773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A135" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M151" sqref="M150:M151"/>
     </sheetView>
   </sheetViews>
@@ -40808,14 +40808,14 @@
         <f t="shared" si="11"/>
         <v>1.4401913875598087</v>
       </c>
-      <c r="G135" s="82" t="s">
+      <c r="G135" s="84" t="s">
         <v>306</v>
       </c>
-      <c r="H135" s="82"/>
-      <c r="I135" s="82"/>
-      <c r="J135" s="82"/>
-      <c r="K135" s="82"/>
-      <c r="L135" s="82"/>
+      <c r="H135" s="84"/>
+      <c r="I135" s="84"/>
+      <c r="J135" s="84"/>
+      <c r="K135" s="84"/>
+      <c r="L135" s="84"/>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="35">
@@ -40835,10 +40835,10 @@
         <f t="shared" ref="E136:E150" si="12">AVERAGE(C134:C136)/AVERAGE(C123:C136)</f>
         <v>1.4455284552845529</v>
       </c>
-      <c r="G136" s="81" t="s">
+      <c r="G136" s="83" t="s">
         <v>308</v>
       </c>
-      <c r="H136" s="81"/>
+      <c r="H136" s="83"/>
       <c r="I136" t="s">
         <v>309</v>
       </c>
@@ -41267,14 +41267,14 @@
         <f t="shared" si="12"/>
         <v>0.8775811209439528</v>
       </c>
-      <c r="G147" s="82" t="s">
+      <c r="G147" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="H147" s="82"/>
-      <c r="I147" s="82"/>
-      <c r="J147" s="82"/>
-      <c r="K147" s="82"/>
-      <c r="L147" s="82"/>
+      <c r="H147" s="84"/>
+      <c r="I147" s="84"/>
+      <c r="J147" s="84"/>
+      <c r="K147" s="84"/>
+      <c r="L147" s="84"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="35">
@@ -41403,7 +41403,7 @@
         <v>13</v>
       </c>
       <c r="D151" s="34">
-        <f t="shared" ref="D142:D151" si="17">AVERAGE(D137:D150)</f>
+        <f t="shared" ref="D151" si="17">AVERAGE(D137:D150)</f>
         <v>2.6869719736727315E-2</v>
       </c>
       <c r="E151" s="34">

</xml_diff>